<commit_message>
Changes on Gen1v2 - refined prompts, refined state
</commit_message>
<xml_diff>
--- a/approaches/evaluation_logs/One_Agent/test-50-evaluation_log-vLLM_kosbu-Llama-3.3-70B-Instruct-AWQ-2025-04-22-0849.xlsx
+++ b/approaches/evaluation_logs/One_Agent/test-50-evaluation_log-vLLM_kosbu-Llama-3.3-70B-Instruct-AWQ-2025-04-22-0849.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U51"/>
+  <dimension ref="A1:W51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,45 +496,55 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Correct Extracted Predicates with Parents</t>
+          <t>Detected Predicates Doc Parent</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Correct Extracted Predicates with Related</t>
+          <t>Detected Predicates Doc Related</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
+          <t>Correct Pred Predicates Parents</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Correct Pred Predicates Related</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
           <t>Extracted Objects</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Gold Standard Objects</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Correct Extracted Objects</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Extracted Entities</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Gold Standard Entities</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Correct Extracted Entities</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Result String</t>
         </is>
@@ -593,15 +603,21 @@
         <v>2</v>
       </c>
       <c r="R2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T2" t="n">
         <v>3</v>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="U2" t="n">
+        <v>3</v>
+      </c>
+      <c r="V2" t="n">
+        <v>3</v>
+      </c>
+      <c r="W2" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -655,24 +671,30 @@
         <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
         <v>2</v>
       </c>
       <c r="R3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T3" t="n">
         <v>3</v>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="U3" t="n">
+        <v>3</v>
+      </c>
+      <c r="V3" t="n">
+        <v>3</v>
+      </c>
+      <c r="W3" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -729,21 +751,27 @@
         <v>2</v>
       </c>
       <c r="P4" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>2</v>
+      </c>
+      <c r="R4" t="n">
         <v>5</v>
       </c>
-      <c r="Q4" t="n">
-        <v>2</v>
-      </c>
-      <c r="R4" t="n">
-        <v>3</v>
-      </c>
       <c r="S4" t="n">
+        <v>2</v>
+      </c>
+      <c r="T4" t="n">
+        <v>3</v>
+      </c>
+      <c r="U4" t="n">
         <v>6</v>
       </c>
-      <c r="T4" t="n">
-        <v>3</v>
-      </c>
-      <c r="U4" t="inlineStr">
+      <c r="V4" t="n">
+        <v>3</v>
+      </c>
+      <c r="W4" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -797,24 +825,30 @@
         <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>4</v>
+      </c>
+      <c r="R5" t="n">
         <v>6</v>
       </c>
-      <c r="Q5" t="n">
-        <v>3</v>
-      </c>
-      <c r="R5" t="n">
+      <c r="S5" t="n">
+        <v>3</v>
+      </c>
+      <c r="T5" t="n">
         <v>5</v>
       </c>
-      <c r="S5" t="n">
+      <c r="U5" t="n">
         <v>7</v>
       </c>
-      <c r="T5" t="n">
-        <v>4</v>
-      </c>
-      <c r="U5" t="inlineStr">
+      <c r="V5" t="n">
+        <v>4</v>
+      </c>
+      <c r="W5" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -872,24 +906,30 @@
         <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>1</v>
-      </c>
-      <c r="U6" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="U6" t="n">
+        <v>2</v>
+      </c>
+      <c r="V6" t="n">
+        <v>1</v>
+      </c>
+      <c r="W6" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -942,24 +982,30 @@
         <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R7" t="n">
         <v>3</v>
       </c>
       <c r="S7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="T7" t="n">
-        <v>2</v>
-      </c>
-      <c r="U7" t="inlineStr">
+        <v>3</v>
+      </c>
+      <c r="U7" t="n">
+        <v>4</v>
+      </c>
+      <c r="V7" t="n">
+        <v>2</v>
+      </c>
+      <c r="W7" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -1023,15 +1069,21 @@
         <v>2</v>
       </c>
       <c r="R8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T8" t="n">
         <v>3</v>
       </c>
-      <c r="U8" t="inlineStr">
+      <c r="U8" t="n">
+        <v>3</v>
+      </c>
+      <c r="V8" t="n">
+        <v>3</v>
+      </c>
+      <c r="W8" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -1085,24 +1137,30 @@
         <v>2</v>
       </c>
       <c r="O9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P9" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>4</v>
+      </c>
+      <c r="R9" t="n">
         <v>6</v>
       </c>
-      <c r="Q9" t="n">
-        <v>2</v>
-      </c>
-      <c r="R9" t="n">
+      <c r="S9" t="n">
+        <v>2</v>
+      </c>
+      <c r="T9" t="n">
         <v>5</v>
       </c>
-      <c r="S9" t="n">
+      <c r="U9" t="n">
         <v>7</v>
       </c>
-      <c r="T9" t="n">
-        <v>3</v>
-      </c>
-      <c r="U9" t="inlineStr">
+      <c r="V9" t="n">
+        <v>3</v>
+      </c>
+      <c r="W9" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -1158,10 +1216,10 @@
         <v>4</v>
       </c>
       <c r="O10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P10" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="Q10" t="n">
         <v>4</v>
@@ -1170,12 +1228,18 @@
         <v>7</v>
       </c>
       <c r="S10" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="T10" t="n">
         <v>7</v>
       </c>
-      <c r="U10" t="inlineStr">
+      <c r="U10" t="n">
+        <v>8</v>
+      </c>
+      <c r="V10" t="n">
+        <v>7</v>
+      </c>
+      <c r="W10" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -1235,21 +1299,27 @@
         <v>2</v>
       </c>
       <c r="P11" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>2</v>
+      </c>
+      <c r="R11" t="n">
         <v>5</v>
       </c>
-      <c r="Q11" t="n">
-        <v>2</v>
-      </c>
-      <c r="R11" t="n">
-        <v>3</v>
-      </c>
       <c r="S11" t="n">
+        <v>2</v>
+      </c>
+      <c r="T11" t="n">
+        <v>3</v>
+      </c>
+      <c r="U11" t="n">
         <v>6</v>
       </c>
-      <c r="T11" t="n">
-        <v>3</v>
-      </c>
-      <c r="U11" t="inlineStr">
+      <c r="V11" t="n">
+        <v>3</v>
+      </c>
+      <c r="W11" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -1306,21 +1376,27 @@
         <v>3</v>
       </c>
       <c r="P12" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>3</v>
+      </c>
+      <c r="R12" t="n">
         <v>5</v>
       </c>
-      <c r="Q12" t="n">
-        <v>3</v>
-      </c>
-      <c r="R12" t="n">
-        <v>4</v>
-      </c>
       <c r="S12" t="n">
+        <v>3</v>
+      </c>
+      <c r="T12" t="n">
+        <v>4</v>
+      </c>
+      <c r="U12" t="n">
         <v>6</v>
       </c>
-      <c r="T12" t="n">
-        <v>4</v>
-      </c>
-      <c r="U12" t="inlineStr">
+      <c r="V12" t="n">
+        <v>4</v>
+      </c>
+      <c r="W12" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -1375,24 +1451,30 @@
         <v>2</v>
       </c>
       <c r="O13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P13" t="n">
         <v>2</v>
       </c>
       <c r="Q13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T13" t="n">
         <v>3</v>
       </c>
-      <c r="U13" t="inlineStr">
+      <c r="U13" t="n">
+        <v>3</v>
+      </c>
+      <c r="V13" t="n">
+        <v>3</v>
+      </c>
+      <c r="W13" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -1449,7 +1531,7 @@
         <v>2</v>
       </c>
       <c r="P14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q14" t="n">
         <v>2</v>
@@ -1458,12 +1540,18 @@
         <v>3</v>
       </c>
       <c r="S14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T14" t="n">
         <v>3</v>
       </c>
-      <c r="U14" t="inlineStr">
+      <c r="U14" t="n">
+        <v>3</v>
+      </c>
+      <c r="V14" t="n">
+        <v>3</v>
+      </c>
+      <c r="W14" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -1517,24 +1605,30 @@
         <v>1</v>
       </c>
       <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="n">
         <v>5</v>
       </c>
-      <c r="P15" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>1</v>
-      </c>
       <c r="R15" t="n">
+        <v>4</v>
+      </c>
+      <c r="S15" t="n">
+        <v>1</v>
+      </c>
+      <c r="T15" t="n">
         <v>7</v>
       </c>
-      <c r="S15" t="n">
+      <c r="U15" t="n">
         <v>5</v>
       </c>
-      <c r="T15" t="n">
-        <v>3</v>
-      </c>
-      <c r="U15" t="inlineStr">
+      <c r="V15" t="n">
+        <v>3</v>
+      </c>
+      <c r="W15" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -1601,15 +1695,21 @@
         <v>1</v>
       </c>
       <c r="R16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T16" t="n">
         <v>2</v>
       </c>
-      <c r="U16" t="inlineStr">
+      <c r="U16" t="n">
+        <v>2</v>
+      </c>
+      <c r="V16" t="n">
+        <v>2</v>
+      </c>
+      <c r="W16" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -1665,7 +1765,7 @@
         <v>2</v>
       </c>
       <c r="P17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q17" t="n">
         <v>2</v>
@@ -1674,12 +1774,18 @@
         <v>3</v>
       </c>
       <c r="S17" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T17" t="n">
         <v>3</v>
       </c>
-      <c r="U17" t="inlineStr">
+      <c r="U17" t="n">
+        <v>4</v>
+      </c>
+      <c r="V17" t="n">
+        <v>3</v>
+      </c>
+      <c r="W17" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -1733,24 +1839,30 @@
         <v>2</v>
       </c>
       <c r="O18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q18" t="n">
         <v>3</v>
       </c>
       <c r="R18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T18" t="n">
         <v>4</v>
       </c>
-      <c r="U18" t="inlineStr">
+      <c r="U18" t="n">
+        <v>4</v>
+      </c>
+      <c r="V18" t="n">
+        <v>4</v>
+      </c>
+      <c r="W18" t="inlineStr">
         <is>
           <t xml:space="preserve">
 &lt;http://www.wikidata.org/entity/Q607380&gt; &lt;http://www.wikidata.org/entity/P183&gt; &lt;http://www.wikidata.org/entity/Q664&gt; .
@@ -1804,24 +1916,30 @@
         <v>2</v>
       </c>
       <c r="O19" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P19" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q19" t="n">
         <v>4</v>
       </c>
       <c r="R19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T19" t="n">
         <v>5</v>
       </c>
-      <c r="U19" t="inlineStr">
+      <c r="U19" t="n">
+        <v>5</v>
+      </c>
+      <c r="V19" t="n">
+        <v>5</v>
+      </c>
+      <c r="W19" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -1877,24 +1995,30 @@
         <v>0</v>
       </c>
       <c r="O20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q20" t="n">
         <v>1</v>
       </c>
       <c r="R20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T20" t="n">
         <v>2</v>
       </c>
-      <c r="U20" t="inlineStr">
+      <c r="U20" t="n">
+        <v>2</v>
+      </c>
+      <c r="V20" t="n">
+        <v>2</v>
+      </c>
+      <c r="W20" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -1950,21 +2074,27 @@
         <v>4</v>
       </c>
       <c r="P21" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>4</v>
+      </c>
+      <c r="R21" t="n">
         <v>7</v>
       </c>
-      <c r="Q21" t="n">
-        <v>4</v>
-      </c>
-      <c r="R21" t="n">
-        <v>6</v>
-      </c>
       <c r="S21" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="T21" t="n">
         <v>6</v>
       </c>
-      <c r="U21" t="inlineStr">
+      <c r="U21" t="n">
+        <v>8</v>
+      </c>
+      <c r="V21" t="n">
+        <v>6</v>
+      </c>
+      <c r="W21" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -2030,15 +2160,21 @@
         <v>1</v>
       </c>
       <c r="R22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T22" t="n">
         <v>2</v>
       </c>
-      <c r="U22" t="inlineStr">
+      <c r="U22" t="n">
+        <v>2</v>
+      </c>
+      <c r="V22" t="n">
+        <v>2</v>
+      </c>
+      <c r="W22" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -2091,24 +2227,30 @@
         <v>2</v>
       </c>
       <c r="O23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q23" t="n">
         <v>3</v>
       </c>
       <c r="R23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T23" t="n">
         <v>4</v>
       </c>
-      <c r="U23" t="inlineStr">
+      <c r="U23" t="n">
+        <v>4</v>
+      </c>
+      <c r="V23" t="n">
+        <v>4</v>
+      </c>
+      <c r="W23" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -2163,24 +2305,30 @@
         <v>1</v>
       </c>
       <c r="O24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q24" t="n">
         <v>2</v>
       </c>
       <c r="R24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T24" t="n">
         <v>3</v>
       </c>
-      <c r="U24" t="inlineStr">
+      <c r="U24" t="n">
+        <v>3</v>
+      </c>
+      <c r="V24" t="n">
+        <v>3</v>
+      </c>
+      <c r="W24" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -2234,24 +2382,30 @@
         <v>2</v>
       </c>
       <c r="O25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q25" t="n">
         <v>3</v>
       </c>
       <c r="R25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T25" t="n">
         <v>4</v>
       </c>
-      <c r="U25" t="inlineStr">
+      <c r="U25" t="n">
+        <v>4</v>
+      </c>
+      <c r="V25" t="n">
+        <v>4</v>
+      </c>
+      <c r="W25" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -2306,24 +2460,30 @@
         <v>1</v>
       </c>
       <c r="O26" t="n">
+        <v>1</v>
+      </c>
+      <c r="P26" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="n">
         <v>8</v>
       </c>
-      <c r="P26" t="n">
+      <c r="R26" t="n">
         <v>7</v>
       </c>
-      <c r="Q26" t="n">
-        <v>4</v>
-      </c>
-      <c r="R26" t="n">
+      <c r="S26" t="n">
+        <v>4</v>
+      </c>
+      <c r="T26" t="n">
         <v>10</v>
       </c>
-      <c r="S26" t="n">
+      <c r="U26" t="n">
         <v>7</v>
       </c>
-      <c r="T26" t="n">
+      <c r="V26" t="n">
         <v>6</v>
       </c>
-      <c r="U26" t="inlineStr">
+      <c r="W26" t="inlineStr">
         <is>
           <t xml:space="preserve">
 &lt;http://www.wikidata.org/entity/Q62066211&gt; &lt;http://www.wikidata.org/entity/P276&gt; &lt;http://www.wikidata.org/entity/Q62066735&gt; .
@@ -2382,24 +2542,30 @@
         <v>1</v>
       </c>
       <c r="O27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P27" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q27" t="n">
         <v>2</v>
       </c>
       <c r="R27" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S27" t="n">
+        <v>2</v>
+      </c>
+      <c r="T27" t="n">
+        <v>3</v>
+      </c>
+      <c r="U27" t="n">
         <v>5</v>
       </c>
-      <c r="T27" t="n">
-        <v>3</v>
-      </c>
-      <c r="U27" t="inlineStr">
+      <c r="V27" t="n">
+        <v>3</v>
+      </c>
+      <c r="W27" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -2462,15 +2628,21 @@
         <v>2</v>
       </c>
       <c r="R28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T28" t="n">
         <v>3</v>
       </c>
-      <c r="U28" t="inlineStr">
+      <c r="U28" t="n">
+        <v>3</v>
+      </c>
+      <c r="V28" t="n">
+        <v>3</v>
+      </c>
+      <c r="W28" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -2524,24 +2696,30 @@
         <v>0</v>
       </c>
       <c r="O29" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q29" t="n">
         <v>6</v>
       </c>
-      <c r="P29" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q29" t="n">
-        <v>4</v>
-      </c>
       <c r="R29" t="n">
+        <v>4</v>
+      </c>
+      <c r="S29" t="n">
+        <v>4</v>
+      </c>
+      <c r="T29" t="n">
         <v>7</v>
       </c>
-      <c r="S29" t="n">
+      <c r="U29" t="n">
         <v>5</v>
       </c>
-      <c r="T29" t="n">
+      <c r="V29" t="n">
         <v>5</v>
       </c>
-      <c r="U29" t="inlineStr">
+      <c r="W29" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -2599,24 +2777,30 @@
         <v>0</v>
       </c>
       <c r="O30" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P30" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q30" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R30" t="n">
+        <v>4</v>
+      </c>
+      <c r="S30" t="n">
+        <v>1</v>
+      </c>
+      <c r="T30" t="n">
         <v>5</v>
       </c>
-      <c r="S30" t="n">
+      <c r="U30" t="n">
         <v>5</v>
       </c>
-      <c r="T30" t="n">
-        <v>2</v>
-      </c>
-      <c r="U30" t="inlineStr">
+      <c r="V30" t="n">
+        <v>2</v>
+      </c>
+      <c r="W30" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wdt: &lt;http://www.wikidata.org/prop/direct/&gt; .
@@ -2673,24 +2857,30 @@
         <v>1</v>
       </c>
       <c r="O31" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P31" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q31" t="n">
         <v>3</v>
       </c>
       <c r="R31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S31" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T31" t="n">
         <v>4</v>
       </c>
-      <c r="U31" t="inlineStr">
+      <c r="U31" t="n">
+        <v>4</v>
+      </c>
+      <c r="V31" t="n">
+        <v>4</v>
+      </c>
+      <c r="W31" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -2746,24 +2936,30 @@
         <v>2</v>
       </c>
       <c r="O32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q32" t="n">
         <v>2</v>
       </c>
       <c r="R32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S32" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T32" t="n">
         <v>3</v>
       </c>
-      <c r="U32" t="inlineStr">
+      <c r="U32" t="n">
+        <v>3</v>
+      </c>
+      <c r="V32" t="n">
+        <v>3</v>
+      </c>
+      <c r="W32" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -2817,24 +3013,30 @@
         <v>2</v>
       </c>
       <c r="O33" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P33" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>4</v>
+      </c>
+      <c r="R33" t="n">
         <v>6</v>
       </c>
-      <c r="Q33" t="n">
-        <v>4</v>
-      </c>
-      <c r="R33" t="n">
-        <v>5</v>
-      </c>
       <c r="S33" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="T33" t="n">
         <v>5</v>
       </c>
-      <c r="U33" t="inlineStr">
+      <c r="U33" t="n">
+        <v>7</v>
+      </c>
+      <c r="V33" t="n">
+        <v>5</v>
+      </c>
+      <c r="W33" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -2890,24 +3092,30 @@
         <v>1</v>
       </c>
       <c r="O34" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P34" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q34" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R34" t="n">
+        <v>3</v>
+      </c>
+      <c r="S34" t="n">
+        <v>3</v>
+      </c>
+      <c r="T34" t="n">
         <v>5</v>
       </c>
-      <c r="S34" t="n">
-        <v>4</v>
-      </c>
-      <c r="T34" t="n">
-        <v>4</v>
-      </c>
-      <c r="U34" t="inlineStr">
+      <c r="U34" t="n">
+        <v>4</v>
+      </c>
+      <c r="V34" t="n">
+        <v>4</v>
+      </c>
+      <c r="W34" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -2969,18 +3177,24 @@
         <v>1</v>
       </c>
       <c r="Q35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S35" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T35" t="n">
         <v>2</v>
       </c>
-      <c r="U35" t="inlineStr">
+      <c r="U35" t="n">
+        <v>2</v>
+      </c>
+      <c r="V35" t="n">
+        <v>2</v>
+      </c>
+      <c r="W35" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -3036,7 +3250,7 @@
         <v>1</v>
       </c>
       <c r="P36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q36" t="n">
         <v>1</v>
@@ -3045,12 +3259,18 @@
         <v>2</v>
       </c>
       <c r="S36" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T36" t="n">
         <v>2</v>
       </c>
-      <c r="U36" t="inlineStr">
+      <c r="U36" t="n">
+        <v>3</v>
+      </c>
+      <c r="V36" t="n">
+        <v>2</v>
+      </c>
+      <c r="W36" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -3103,24 +3323,30 @@
         <v>2</v>
       </c>
       <c r="O37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q37" t="n">
         <v>3</v>
       </c>
       <c r="R37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T37" t="n">
         <v>4</v>
       </c>
-      <c r="U37" t="inlineStr">
+      <c r="U37" t="n">
+        <v>4</v>
+      </c>
+      <c r="V37" t="n">
+        <v>4</v>
+      </c>
+      <c r="W37" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -3175,24 +3401,30 @@
         <v>0</v>
       </c>
       <c r="O38" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P38" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q38" t="n">
         <v>4</v>
       </c>
       <c r="R38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T38" t="n">
         <v>5</v>
       </c>
-      <c r="U38" t="inlineStr">
+      <c r="U38" t="n">
+        <v>5</v>
+      </c>
+      <c r="V38" t="n">
+        <v>5</v>
+      </c>
+      <c r="W38" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -3258,15 +3490,21 @@
         <v>2</v>
       </c>
       <c r="R39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T39" t="n">
         <v>3</v>
       </c>
-      <c r="U39" t="inlineStr">
+      <c r="U39" t="n">
+        <v>3</v>
+      </c>
+      <c r="V39" t="n">
+        <v>3</v>
+      </c>
+      <c r="W39" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -3320,24 +3558,30 @@
         <v>1</v>
       </c>
       <c r="O40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P40" t="n">
         <v>1</v>
       </c>
       <c r="Q40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T40" t="n">
         <v>2</v>
       </c>
-      <c r="U40" t="inlineStr">
+      <c r="U40" t="n">
+        <v>2</v>
+      </c>
+      <c r="V40" t="n">
+        <v>2</v>
+      </c>
+      <c r="W40" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -3400,15 +3644,21 @@
         <v>2</v>
       </c>
       <c r="R41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T41" t="n">
         <v>3</v>
       </c>
-      <c r="U41" t="inlineStr">
+      <c r="U41" t="n">
+        <v>3</v>
+      </c>
+      <c r="V41" t="n">
+        <v>3</v>
+      </c>
+      <c r="W41" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -3456,16 +3706,16 @@
         <v>3</v>
       </c>
       <c r="M42" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N42" t="n">
         <v>4</v>
       </c>
       <c r="O42" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P42" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="Q42" t="n">
         <v>5</v>
@@ -3474,12 +3724,18 @@
         <v>6</v>
       </c>
       <c r="S42" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="T42" t="n">
         <v>6</v>
       </c>
-      <c r="U42" t="inlineStr">
+      <c r="U42" t="n">
+        <v>7</v>
+      </c>
+      <c r="V42" t="n">
+        <v>6</v>
+      </c>
+      <c r="W42" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -3536,24 +3792,30 @@
         <v>1</v>
       </c>
       <c r="O43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q43" t="n">
         <v>2</v>
       </c>
       <c r="R43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S43" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T43" t="n">
         <v>3</v>
       </c>
-      <c r="U43" t="inlineStr">
+      <c r="U43" t="n">
+        <v>3</v>
+      </c>
+      <c r="V43" t="n">
+        <v>3</v>
+      </c>
+      <c r="W43" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -3609,24 +3871,30 @@
         <v>0</v>
       </c>
       <c r="O44" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P44" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q44" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R44" t="n">
         <v>2</v>
       </c>
       <c r="S44" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T44" t="n">
-        <v>1</v>
-      </c>
-      <c r="U44" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="U44" t="n">
+        <v>3</v>
+      </c>
+      <c r="V44" t="n">
+        <v>1</v>
+      </c>
+      <c r="W44" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -3681,24 +3949,30 @@
         <v>0</v>
       </c>
       <c r="O45" t="n">
+        <v>0</v>
+      </c>
+      <c r="P45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q45" t="n">
         <v>7</v>
       </c>
-      <c r="P45" t="n">
+      <c r="R45" t="n">
         <v>9</v>
       </c>
-      <c r="Q45" t="n">
-        <v>3</v>
-      </c>
-      <c r="R45" t="n">
+      <c r="S45" t="n">
+        <v>3</v>
+      </c>
+      <c r="T45" t="n">
         <v>8</v>
       </c>
-      <c r="S45" t="n">
+      <c r="U45" t="n">
         <v>10</v>
       </c>
-      <c r="T45" t="n">
-        <v>4</v>
-      </c>
-      <c r="U45" t="inlineStr">
+      <c r="V45" t="n">
+        <v>4</v>
+      </c>
+      <c r="W45" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wdt: &lt;http://www.wikidata.org/prop/direct/&gt; .
@@ -3758,24 +4032,30 @@
         <v>0</v>
       </c>
       <c r="O46" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P46" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q46" t="n">
         <v>3</v>
       </c>
       <c r="R46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T46" t="n">
         <v>4</v>
       </c>
-      <c r="U46" t="inlineStr">
+      <c r="U46" t="n">
+        <v>4</v>
+      </c>
+      <c r="V46" t="n">
+        <v>4</v>
+      </c>
+      <c r="W46" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -3835,21 +4115,27 @@
         <v>1</v>
       </c>
       <c r="P47" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q47" t="n">
         <v>1</v>
       </c>
       <c r="R47" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S47" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="T47" t="n">
         <v>2</v>
       </c>
-      <c r="U47" t="inlineStr">
+      <c r="U47" t="n">
+        <v>4</v>
+      </c>
+      <c r="V47" t="n">
+        <v>2</v>
+      </c>
+      <c r="W47" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -3911,15 +4197,21 @@
         <v>2</v>
       </c>
       <c r="R48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T48" t="n">
         <v>3</v>
       </c>
-      <c r="U48" t="inlineStr">
+      <c r="U48" t="n">
+        <v>3</v>
+      </c>
+      <c r="V48" t="n">
+        <v>3</v>
+      </c>
+      <c r="W48" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -3974,24 +4266,30 @@
         <v>3</v>
       </c>
       <c r="O49" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P49" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>4</v>
+      </c>
+      <c r="R49" t="n">
         <v>6</v>
       </c>
-      <c r="Q49" t="n">
-        <v>2</v>
-      </c>
-      <c r="R49" t="n">
+      <c r="S49" t="n">
+        <v>2</v>
+      </c>
+      <c r="T49" t="n">
         <v>5</v>
       </c>
-      <c r="S49" t="n">
+      <c r="U49" t="n">
         <v>7</v>
       </c>
-      <c r="T49" t="n">
-        <v>3</v>
-      </c>
-      <c r="U49" t="inlineStr">
+      <c r="V49" t="n">
+        <v>3</v>
+      </c>
+      <c r="W49" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -4048,24 +4346,30 @@
         <v>2</v>
       </c>
       <c r="O50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q50" t="n">
         <v>3</v>
       </c>
       <c r="R50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T50" t="n">
         <v>4</v>
       </c>
-      <c r="U50" t="inlineStr">
+      <c r="U50" t="n">
+        <v>4</v>
+      </c>
+      <c r="V50" t="n">
+        <v>4</v>
+      </c>
+      <c r="W50" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .
@@ -4129,15 +4433,21 @@
         <v>1</v>
       </c>
       <c r="R51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T51" t="n">
         <v>2</v>
       </c>
-      <c r="U51" t="inlineStr">
+      <c r="U51" t="n">
+        <v>2</v>
+      </c>
+      <c r="V51" t="n">
+        <v>2</v>
+      </c>
+      <c r="W51" t="inlineStr">
         <is>
           <t xml:space="preserve">
 @prefix wd: &lt;http://www.wikidata.org/entity/&gt; .

</xml_diff>